<commit_message>
Change material name for concept where it is required
</commit_message>
<xml_diff>
--- a/src/assets/documents/FORMATO_VOLUMETRIA.xlsx
+++ b/src/assets/documents/FORMATO_VOLUMETRIA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemo/Projects/bellarti-app/src/assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82254B53-8FE4-514D-838E-B1476580A5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F118EFE5-DC9A-584D-9C8D-32A2BAB4F522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="500" windowWidth="25600" windowHeight="26500" xr2:uid="{A2E6BAD1-0106-5E40-8C01-4E780781C887}"/>
   </bookViews>
@@ -36,15 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>MATERIAL</t>
-  </si>
-  <si>
     <t>REFERENCIA</t>
   </si>
   <si>
-    <t>UNIDAD</t>
-  </si>
-  <si>
     <t>CLOSET 1 - FÁBRICA</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>COCINA - INSTALACIÓN</t>
   </si>
   <si>
-    <t>CÓDIGO INTERNO</t>
-  </si>
-  <si>
     <t>REPISA DE BAÑO - FÁBRICA</t>
   </si>
   <si>
@@ -94,6 +85,15 @@
   </si>
   <si>
     <t>PUERTAS DE INTERCOMUNICACIÓN - INSTALACIÓN</t>
+  </si>
+  <si>
+    <t>UNIDAD DE MEDIDA</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CONCEPTO MATERIAL</t>
   </si>
 </sst>
 </file>
@@ -524,13 +524,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="92" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C8" sqref="C8"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -553,64 +553,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update volumetry process - kitchen prototype include
</commit_message>
<xml_diff>
--- a/src/assets/documents/FORMATO_VOLUMETRIA.xlsx
+++ b/src/assets/documents/FORMATO_VOLUMETRIA.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemo/Projects/bellarti-app/src/assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F118EFE5-DC9A-584D-9C8D-32A2BAB4F522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF249FD-5254-9743-AF42-A6655B150199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="25600" windowHeight="26500" xr2:uid="{A2E6BAD1-0106-5E40-8C01-4E780781C887}"/>
+    <workbookView xWindow="-25680" yWindow="960" windowWidth="25600" windowHeight="26500" xr2:uid="{A2E6BAD1-0106-5E40-8C01-4E780781C887}"/>
   </bookViews>
   <sheets>
-    <sheet name="NOMBRE_PROTOTIPO" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,59 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>REFERENCIA</t>
   </si>
   <si>
-    <t>CLOSET 1 - FÁBRICA</t>
-  </si>
-  <si>
-    <t>CLOSET 1 - INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>CLOSET 2 - FÁBRICA</t>
-  </si>
-  <si>
-    <t>CLOSET 2 - INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>VESTIDOR - FÁBRICA</t>
-  </si>
-  <si>
-    <t>VESTIDOR - INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>MUEBLES DE BAÑO PPAL - FÁBRICA</t>
-  </si>
-  <si>
-    <t>MUEBLES DE BAÑO PPAL - INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>MUEBLE DE BAÑO SEC - FÁBRICA</t>
-  </si>
-  <si>
-    <t>MUEBLE DE BAÑO SEC - INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>COCINA - FÁBRICA</t>
-  </si>
-  <si>
-    <t>COCINA - INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>REPISA DE BAÑO - FÁBRICA</t>
-  </si>
-  <si>
-    <t>REPISA DE BAÑO - INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>PUERTAS DE INTERCOMUNICACIÓN - FÁBRICA</t>
-  </si>
-  <si>
-    <t>PUERTAS DE INTERCOMUNICACIÓN - INSTALACIÓN</t>
-  </si>
-  <si>
     <t>UNIDAD DE MEDIDA</t>
   </si>
   <si>
@@ -94,6 +46,33 @@
   </si>
   <si>
     <t xml:space="preserve"> CONCEPTO MATERIAL</t>
+  </si>
+  <si>
+    <t>CLOSET</t>
+  </si>
+  <si>
+    <t>FÁBRICA</t>
+  </si>
+  <si>
+    <t>INSTALACIÓN</t>
+  </si>
+  <si>
+    <t>CLOSET 2</t>
+  </si>
+  <si>
+    <t>VESTIDOR</t>
+  </si>
+  <si>
+    <t>MUEBLES DE BAÑO PPAL</t>
+  </si>
+  <si>
+    <t>MUEBLE DE BAÑO SEC</t>
+  </si>
+  <si>
+    <t>REPISA DE BAÑO</t>
+  </si>
+  <si>
+    <t>PUERTAS DE INTERCOMUNICACIÓN</t>
   </si>
 </sst>
 </file>
@@ -131,23 +110,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -157,31 +125,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -191,20 +137,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,100 +465,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FC5A6A-CCAD-7248-A7FF-3E2CEE82B19E}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="92" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K1" sqref="K1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.6640625" customWidth="1"/>
-    <col min="15" max="15" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.83203125" customWidth="1"/>
-    <col min="18" max="18" width="29.33203125" customWidth="1"/>
-    <col min="19" max="19" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="9.83203125" customWidth="1"/>
+    <col min="16" max="16" width="13.5" customWidth="1"/>
+    <col min="17" max="17" width="16.5" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="R1" s="2"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>16</v>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Purchase order changes - second step
</commit_message>
<xml_diff>
--- a/src/assets/documents/FORMATO_VOLUMETRIA.xlsx
+++ b/src/assets/documents/FORMATO_VOLUMETRIA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemo/Projects/bellarti-app/src/assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF249FD-5254-9743-AF42-A6655B150199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348A50E0-9019-5F4C-840E-99C6229061EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25680" yWindow="960" windowWidth="25600" windowHeight="26500" xr2:uid="{A2E6BAD1-0106-5E40-8C01-4E780781C887}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
-  <si>
-    <t>REFERENCIA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>UNIDAD DE MEDIDA</t>
   </si>
@@ -465,11 +462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FC5A6A-CCAD-7248-A7FF-3E2CEE82B19E}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="92" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1:L1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,126 +474,120 @@
     <col min="1" max="1" width="46.5" customWidth="1"/>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" customWidth="1"/>
-    <col min="16" max="16" width="13.5" customWidth="1"/>
-    <col min="17" max="17" width="16.5" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="9.83203125" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="16" width="16.5" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="G1:H1"/>
+  <mergeCells count="10">
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="F1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>